<commit_message>
Modificacion del archivo de requerimientos
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de trabajo - Hotel.xlsx
+++ b/Documentacion/Plan de trabajo - Hotel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis501Angel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis501Angel\Documents\Github\Proyecto hotel\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6068CA08-5804-41D6-9318-199B2BCB0DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4FCE84-9531-45B8-A170-A0F806A150B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{68151F5F-C06A-4AA8-9BD5-751EF5558B1B}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{68151F5F-C06A-4AA8-9BD5-751EF5558B1B}"/>
   </bookViews>
   <sheets>
     <sheet name="WBSData" sheetId="2" r:id="rId1"/>
@@ -1074,9 +1074,6 @@
     <t>Inicia</t>
   </si>
   <si>
-    <t xml:space="preserve">Luis Romero </t>
-  </si>
-  <si>
     <t>Aldo Diaz</t>
   </si>
   <si>
@@ -1084,15 +1081,17 @@
   </si>
   <si>
     <t>Luis Romero, Daniel Nolasco, Aldo Diaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luis Romero, Daniel Nolasco, Aldo Diaz, Ibet Ortiz </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1165,13 +1164,13 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1193,7 +1192,7 @@
       <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1518,10 +1517,10 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" outlineLevelRow="4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
@@ -1529,7 +1528,7 @@
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="37.77734375" customWidth="1"/>
     <col min="8" max="8" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="33.109375" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1659,7 +1658,7 @@
         <v>43913</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -1711,7 +1710,7 @@
         <v>43916</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -1737,7 +1736,7 @@
         <v>43920</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1789,7 +1788,7 @@
         <v>43921</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1815,7 +1814,7 @@
         <v>43934</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1841,7 +1840,7 @@
         <v>43934</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1867,7 +1866,7 @@
         <v>43934</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -2098,7 +2097,7 @@
       <selection sqref="A1:IE24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:239" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Modificaciones a los documentos
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de trabajo - Hotel.xlsx
+++ b/Documentacion/Plan de trabajo - Hotel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis501Angel\Documents\Github\Proyecto hotel\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4FCE84-9531-45B8-A170-A0F806A150B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98545BD8-6250-46E2-A37A-F4576ABDA457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{68151F5F-C06A-4AA8-9BD5-751EF5558B1B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="352">
   <si>
     <t>Work-</t>
   </si>
@@ -1084,6 +1084,12 @@
   </si>
   <si>
     <t xml:space="preserve">Luis Romero, Daniel Nolasco, Aldo Diaz, Ibet Ortiz </t>
+  </si>
+  <si>
+    <t>Mockups</t>
+  </si>
+  <si>
+    <t>Daniel Trujillo</t>
   </si>
 </sst>
 </file>
@@ -1517,7 +1523,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" outlineLevelRow="4" x14ac:dyDescent="0.3"/>
@@ -1626,13 +1632,13 @@
         <v>320</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>266</v>
+        <v>350</v>
       </c>
       <c r="H4" s="24">
-        <v>43909</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>336</v>
+        <v>43908</v>
+      </c>
+      <c r="I4" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -1652,13 +1658,13 @@
         <v>320</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>337</v>
+        <v>266</v>
       </c>
       <c r="H5" s="24">
-        <v>43913</v>
+        <v>43909</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -1678,13 +1684,13 @@
         <v>320</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>279</v>
+        <v>337</v>
       </c>
       <c r="H6" s="24">
         <v>43913</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1703,14 +1709,14 @@
       <c r="E7" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>338</v>
-      </c>
-      <c r="H7" s="23">
-        <v>43916</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>346</v>
+      <c r="G7" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="H7" s="24">
+        <v>43913</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -1730,13 +1736,13 @@
         <v>327</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H8" s="23">
-        <v>43920</v>
+        <v>43916</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1756,13 +1762,13 @@
         <v>320</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>289</v>
+        <v>339</v>
       </c>
       <c r="H9" s="23">
         <v>43920</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" spans="1:9" outlineLevel="4" x14ac:dyDescent="0.3">
@@ -1781,14 +1787,14 @@
       <c r="E10" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="H10" s="24">
-        <v>43921</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>346</v>
+      <c r="G10" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="H10" s="23">
+        <v>43920</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1808,13 +1814,13 @@
         <v>320</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>270</v>
+        <v>340</v>
       </c>
       <c r="H11" s="24">
-        <v>43934</v>
+        <v>43921</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1834,7 +1840,7 @@
         <v>320</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="H12" s="24">
         <v>43934</v>
@@ -1860,7 +1866,7 @@
         <v>320</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="H13" s="24">
         <v>43934</v>
@@ -1885,14 +1891,14 @@
       <c r="E14" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="G14" s="22" t="s">
-        <v>341</v>
-      </c>
-      <c r="H14" s="23">
-        <v>43935</v>
-      </c>
-      <c r="I14" s="22" t="s">
-        <v>334</v>
+      <c r="G14" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H14" s="24">
+        <v>43934</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1911,8 +1917,8 @@
       <c r="E15" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="G15" s="25" t="s">
-        <v>342</v>
+      <c r="G15" s="22" t="s">
+        <v>341</v>
       </c>
       <c r="H15" s="23">
         <v>43935</v>
@@ -1938,7 +1944,7 @@
         <v>320</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H16" s="23">
         <v>43935</v>
@@ -1947,7 +1953,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>295</v>
       </c>
@@ -1963,8 +1969,17 @@
       <c r="E17" s="12" t="s">
         <v>326</v>
       </c>
+      <c r="G17" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="H17" s="23">
+        <v>43935</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>334</v>
+      </c>
     </row>
-    <row r="18" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>298</v>
       </c>
@@ -1981,7 +1996,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="19" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>300</v>
       </c>
@@ -1998,7 +2013,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="20" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>303</v>
       </c>
@@ -2015,7 +2030,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>305</v>
       </c>
@@ -2032,7 +2047,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="22" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>309</v>
       </c>
@@ -2049,7 +2064,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>313</v>
       </c>
@@ -2066,7 +2081,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>316</v>
       </c>

</xml_diff>

<commit_message>
Agregue plan de trabajo en PDF
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de trabajo - Hotel.xlsx
+++ b/Documentacion/Plan de trabajo - Hotel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dniel\Documents\ProyectoHotel\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis501Angel\Documents\Github\Proyecto hotel\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46025E43-1DD3-4EA8-B17B-B690AC536BD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ABC6CD-248F-43A9-B873-78306327A988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{68151F5F-C06A-4AA8-9BD5-751EF5558B1B}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{68151F5F-C06A-4AA8-9BD5-751EF5558B1B}"/>
   </bookViews>
   <sheets>
     <sheet name="WBSData" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1159,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1199,7 +1201,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1520,10 +1521,10 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" outlineLevelRow="4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
@@ -1534,7 +1535,7 @@
     <col min="9" max="9" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.55" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>317</v>
       </c>
@@ -1560,7 +1561,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="14.55" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>241</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" ht="14.55" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>254</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>258</v>
       </c>
@@ -1637,11 +1638,11 @@
         <f>D6</f>
         <v>43913.708333333336</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="26" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>264</v>
       </c>
@@ -1668,7 +1669,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>267</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" ht="14.55" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>269</v>
       </c>
@@ -1722,7 +1723,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>271</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" ht="14.55" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="6" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>275</v>
       </c>
@@ -1776,7 +1777,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="10" spans="1:9" outlineLevel="4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.4" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>278</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.55" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>280</v>
       </c>
@@ -1830,7 +1831,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.55" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>283</v>
       </c>
@@ -1857,7 +1858,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.55" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>286</v>
       </c>
@@ -1884,7 +1885,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>288</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.55" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>290</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.55" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>293</v>
       </c>
@@ -1965,7 +1966,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="6" customFormat="1" ht="14.55" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>295</v>
       </c>
@@ -1992,7 +1993,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="18" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.4" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>298</v>
       </c>
@@ -2009,7 +2010,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>300</v>
       </c>
@@ -2026,7 +2027,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>303</v>
       </c>
@@ -2043,7 +2044,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="6" customFormat="1" ht="14.55" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>305</v>
       </c>
@@ -2060,7 +2061,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>309</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>313</v>
       </c>
@@ -2094,7 +2095,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.55" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>316</v>
       </c>
@@ -2125,7 +2126,7 @@
       <selection sqref="A1:IE24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:239" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Plan de trabajo modificado - Actualizacion de fechas
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de trabajo - Hotel.xlsx
+++ b/Documentacion/Plan de trabajo - Hotel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis501Angel\Documents\Github\Proyecto hotel\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ABC6CD-248F-43A9-B873-78306327A988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC89E9E-D061-4162-966F-E001CF138A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{68151F5F-C06A-4AA8-9BD5-751EF5558B1B}"/>
   </bookViews>
@@ -1521,7 +1521,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" outlineLevelRow="4" x14ac:dyDescent="0.3"/>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="H12" s="24">
         <f>D18</f>
-        <v>43929.708333333336</v>
+        <v>43946.708333333336</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>344</v>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="H13" s="24">
         <f t="shared" ref="H13:H14" si="1">D19</f>
-        <v>43933.708333333336</v>
+        <v>43950.708333333336</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>344</v>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="H14" s="24">
         <f t="shared" si="1"/>
-        <v>43937.708333333336</v>
+        <v>43954.708333333336</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>344</v>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="H15" s="23">
         <f>D22</f>
-        <v>43938.708333333336</v>
+        <v>43954.708333333336</v>
       </c>
       <c r="I15" s="22" t="s">
         <v>331</v>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="H16" s="23">
         <f t="shared" ref="H16:H17" si="2">D23</f>
-        <v>43939</v>
+        <v>43955</v>
       </c>
       <c r="I16" s="22" t="s">
         <v>331</v>
@@ -1977,7 +1977,7 @@
         <v>43926.541666666664</v>
       </c>
       <c r="D17" s="11">
-        <v>43937.708333333336</v>
+        <v>43954.708333333336</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>324</v>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="H17" s="23">
         <f t="shared" si="2"/>
-        <v>43940</v>
+        <v>43956</v>
       </c>
       <c r="I17" s="22" t="s">
         <v>331</v>
@@ -2001,10 +2001,10 @@
         <v>270</v>
       </c>
       <c r="C18" s="23">
-        <v>43926.541666666664</v>
+        <v>43943.541666666664</v>
       </c>
       <c r="D18" s="8">
-        <v>43929.708333333336</v>
+        <v>43946.708333333336</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>322</v>
@@ -2018,10 +2018,10 @@
         <v>287</v>
       </c>
       <c r="C19" s="8">
-        <v>43930.541666666664</v>
+        <v>43947.541666666664</v>
       </c>
       <c r="D19" s="8">
-        <v>43933.708333333336</v>
+        <v>43950.708333333336</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>322</v>
@@ -2035,10 +2035,10 @@
         <v>302</v>
       </c>
       <c r="C20" s="8">
-        <v>43934.541666666664</v>
+        <v>43951.541666666664</v>
       </c>
       <c r="D20" s="8">
-        <v>43937.708333333336</v>
+        <v>43954.708333333336</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>322</v>
@@ -2052,7 +2052,7 @@
         <v>304</v>
       </c>
       <c r="C21" s="11">
-        <v>43938.541666666664</v>
+        <v>43954.541666666664</v>
       </c>
       <c r="D21" s="11">
         <v>43940.708333333336</v>
@@ -2069,10 +2069,10 @@
         <v>308</v>
       </c>
       <c r="C22" s="8">
-        <v>43938.541666666664</v>
+        <v>43954.541666666664</v>
       </c>
       <c r="D22" s="8">
-        <v>43938.708333333336</v>
+        <v>43954.708333333336</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>323</v>
@@ -2086,10 +2086,10 @@
         <v>312</v>
       </c>
       <c r="C23" s="24">
-        <v>43939</v>
+        <v>43955</v>
       </c>
       <c r="D23" s="24">
-        <v>43939</v>
+        <v>43955</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>323</v>
@@ -2103,10 +2103,10 @@
         <v>315</v>
       </c>
       <c r="C24" s="24">
-        <v>43940</v>
+        <v>43956</v>
       </c>
       <c r="D24" s="24">
-        <v>43940</v>
+        <v>43956</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>323</v>

</xml_diff>

<commit_message>
Plan de trabajo modificado - Actualizacion de fechas de pruebas
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de trabajo - Hotel.xlsx
+++ b/Documentacion/Plan de trabajo - Hotel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis501Angel\Documents\Github\Proyecto hotel\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC89E9E-D061-4162-966F-E001CF138A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE704CC-997C-4D54-B7E9-950F4AA7611C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{68151F5F-C06A-4AA8-9BD5-751EF5558B1B}"/>
   </bookViews>
@@ -1521,7 +1521,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" outlineLevelRow="4" x14ac:dyDescent="0.3"/>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="H15" s="23">
         <f>D22</f>
-        <v>43954.708333333336</v>
+        <v>43955.708333333336</v>
       </c>
       <c r="I15" s="22" t="s">
         <v>331</v>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="H16" s="23">
         <f t="shared" ref="H16:H17" si="2">D23</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="I16" s="22" t="s">
         <v>331</v>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="H17" s="23">
         <f t="shared" si="2"/>
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="I17" s="22" t="s">
         <v>331</v>
@@ -2069,10 +2069,10 @@
         <v>308</v>
       </c>
       <c r="C22" s="8">
-        <v>43954.541666666664</v>
+        <v>43955.541666666664</v>
       </c>
       <c r="D22" s="8">
-        <v>43954.708333333336</v>
+        <v>43955.708333333336</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>323</v>
@@ -2086,10 +2086,10 @@
         <v>312</v>
       </c>
       <c r="C23" s="24">
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="D23" s="24">
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>323</v>
@@ -2103,10 +2103,10 @@
         <v>315</v>
       </c>
       <c r="C24" s="24">
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="D24" s="24">
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>323</v>

</xml_diff>

<commit_message>
Plan de trabajo actualizado
</commit_message>
<xml_diff>
--- a/Documentacion/Plan de trabajo - Hotel.xlsx
+++ b/Documentacion/Plan de trabajo - Hotel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis501Angel\Documents\Github\Proyecto hotel\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis501Angel\Documents\Github\ProyectoHotel\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE704CC-997C-4D54-B7E9-950F4AA7611C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702C0E08-F6C0-49F4-8F60-BAF87227553E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{68151F5F-C06A-4AA8-9BD5-751EF5558B1B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="356">
   <si>
     <t>Work-</t>
   </si>
@@ -1087,6 +1087,21 @@
   </si>
   <si>
     <t>6 dias + 5 (restraso)</t>
+  </si>
+  <si>
+    <t>Demo 1</t>
+  </si>
+  <si>
+    <t>Demo 2</t>
+  </si>
+  <si>
+    <t>Luis Romero, Daniel Nolasco, Aldo Diaz, Ibet Ortiz , Daniel Trujillo</t>
+  </si>
+  <si>
+    <t>Demo 3</t>
+  </si>
+  <si>
+    <t>Demo 4</t>
   </si>
 </sst>
 </file>
@@ -1521,7 +1536,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" outlineLevelRow="4" x14ac:dyDescent="0.3"/>
@@ -1532,7 +1547,7 @@
     <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37.77734375" customWidth="1"/>
     <col min="8" max="8" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="41.109375" customWidth="1"/>
+    <col min="9" max="9" width="54.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1716,7 +1731,7 @@
         <v>279</v>
       </c>
       <c r="H7" s="24">
-        <f t="shared" ref="H7:H9" si="0">D11</f>
+        <f t="shared" ref="H7" si="0">D11</f>
         <v>43917.708333333336</v>
       </c>
       <c r="I7" s="7" t="s">
@@ -1743,7 +1758,7 @@
         <v>334</v>
       </c>
       <c r="H8" s="24">
-        <f t="shared" si="0"/>
+        <f>D12</f>
         <v>43919.708333333336</v>
       </c>
       <c r="I8" s="22" t="s">
@@ -1770,14 +1785,14 @@
         <v>335</v>
       </c>
       <c r="H9" s="24">
-        <f t="shared" si="0"/>
+        <f>D13</f>
         <v>43921.708333333336</v>
       </c>
       <c r="I9" s="22" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.4" outlineLevel="4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>278</v>
       </c>
@@ -1848,14 +1863,13 @@
         <v>320</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>270</v>
+        <v>351</v>
       </c>
       <c r="H12" s="24">
-        <f>D18</f>
-        <v>43946.708333333336</v>
+        <v>43981</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1875,14 +1889,13 @@
         <v>320</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>287</v>
+        <v>352</v>
       </c>
       <c r="H13" s="24">
-        <f t="shared" ref="H13:H14" si="1">D19</f>
-        <v>43950.708333333336</v>
+        <v>44010</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -1901,15 +1914,14 @@
       <c r="E14" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="H14" s="24">
-        <f t="shared" si="1"/>
-        <v>43954.708333333336</v>
+      <c r="G14" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="H14" s="23">
+        <v>44024</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
     </row>
     <row r="15" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1928,15 +1940,14 @@
       <c r="E15" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="G15" s="22" t="s">
-        <v>337</v>
+      <c r="G15" s="7" t="s">
+        <v>355</v>
       </c>
       <c r="H15" s="23">
-        <f>D22</f>
-        <v>43955.708333333336</v>
-      </c>
-      <c r="I15" s="22" t="s">
-        <v>331</v>
+        <v>44024</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.3">
@@ -1955,15 +1966,15 @@
       <c r="E16" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="G16" s="25" t="s">
-        <v>338</v>
-      </c>
-      <c r="H16" s="23">
-        <f t="shared" ref="H16:H17" si="2">D23</f>
-        <v>43956</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>331</v>
+      <c r="G16" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="H16" s="24">
+        <f>D18</f>
+        <v>44032.708333333336</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1982,18 +1993,18 @@
       <c r="E17" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="G17" s="25" t="s">
-        <v>339</v>
-      </c>
-      <c r="H17" s="23">
-        <f t="shared" si="2"/>
-        <v>43957</v>
-      </c>
-      <c r="I17" s="22" t="s">
-        <v>331</v>
+      <c r="G17" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="H17" s="24">
+        <f>D19</f>
+        <v>44032.708333333336</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>344</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.4" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>298</v>
       </c>
@@ -2004,10 +2015,20 @@
         <v>43943.541666666664</v>
       </c>
       <c r="D18" s="8">
-        <v>43946.708333333336</v>
+        <v>44032.708333333336</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>322</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H18" s="24">
+        <f>D20</f>
+        <v>44032.708333333336</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -2020,11 +2041,21 @@
       <c r="C19" s="8">
         <v>43947.541666666664</v>
       </c>
-      <c r="D19" s="8">
-        <v>43950.708333333336</v>
+      <c r="D19" s="24">
+        <v>44032.708333333336</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>322</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="H19" s="23">
+        <f>D22</f>
+        <v>44035.541666666664</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -2037,11 +2068,21 @@
       <c r="C20" s="8">
         <v>43951.541666666664</v>
       </c>
-      <c r="D20" s="8">
-        <v>43954.708333333336</v>
+      <c r="D20" s="24">
+        <v>44032.708333333336</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>322</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="H20" s="23">
+        <f>D23</f>
+        <v>44035.541666666664</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2060,6 +2101,16 @@
       <c r="E21" s="12" t="s">
         <v>321</v>
       </c>
+      <c r="G21" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="H21" s="23">
+        <f>D24</f>
+        <v>44035.541666666664</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="22" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
@@ -2069,10 +2120,10 @@
         <v>308</v>
       </c>
       <c r="C22" s="8">
-        <v>43955.541666666664</v>
-      </c>
-      <c r="D22" s="8">
-        <v>43955.708333333336</v>
+        <v>44035.541666666664</v>
+      </c>
+      <c r="D22" s="24">
+        <v>44035.541666666664</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>323</v>
@@ -2086,10 +2137,10 @@
         <v>312</v>
       </c>
       <c r="C23" s="24">
-        <v>43956</v>
+        <v>44035.541666666664</v>
       </c>
       <c r="D23" s="24">
-        <v>43956</v>
+        <v>44035.541666666664</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>323</v>
@@ -2103,10 +2154,10 @@
         <v>315</v>
       </c>
       <c r="C24" s="24">
-        <v>43957</v>
+        <v>44035.541666666664</v>
       </c>
       <c r="D24" s="24">
-        <v>43957</v>
+        <v>44035.541666666664</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>323</v>

</xml_diff>